<commit_message>
Uma penca de coisa, principalmente com o articy
</commit_message>
<xml_diff>
--- a/Assets/loc_All objects_en.xlsx
+++ b/Assets/loc_All objects_en.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="339">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="359">
   <x:si>
     <x:t>LocaID</x:t>
   </x:si>
@@ -31,10 +31,10 @@
     <x:t>FFr_C9C294A8.DisplayName</x:t>
   </x:si>
   <x:si>
-    <x:t>Untitled flow fragment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Flow/Untitled flow fragment</x:t>
+    <x:t>Start Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flow/Start Point</x:t>
   </x:si>
   <x:si>
     <x:t>FFr_C9C294A8.Text</x:t>
@@ -454,7 +454,7 @@
     <x:t>Dlg_3EB04445.Text</x:t>
   </x:si>
   <x:si>
-    <x:t>Meu irmão, Ganart, está no pátio de treinamento. Irei desafia-lo.</x:t>
+    <x:t>Meu irmão,  &lt;color=#ffa61aff&gt;Jorrei&lt;/color&gt;, está no pátio de treinamento. Irei desafia-lo.</x:t>
   </x:si>
   <x:si>
     <x:t>Dlg_EE0B5AAB.DisplayName</x:t>
@@ -475,10 +475,10 @@
     <x:t>Dlg_14D539F1.DisplayName</x:t>
   </x:si>
   <x:si>
-    <x:t>Untitled dialogue (03)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Flow/Untitled dialogue (03)</x:t>
+    <x:t>omenor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flow/omenor</x:t>
   </x:si>
   <x:si>
     <x:t>Dlg_14D539F1.Text</x:t>
@@ -1013,6 +1013,45 @@
     <x:t>Não há nada de interessante aqui, quando construiram nosso castelo devem ter movido tudo de importante para lá. Nosso pai só deve vir aqui pelo altar e pela nossa história.</x:t>
   </x:si>
   <x:si>
+    <x:t>m_Minotaur.DisplayName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Minotaur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entities/Characters/Minotaur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_Minotaur.Text</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_Minotaur.DefaultBasicCharacterFeature.Species</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_Jorrah.DisplayName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jorrei</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entities/Characters/Jorrei</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_Jorrah.Text</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_Teste.DisplayName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Teste</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entities/Characters/Teste</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_Teste.Text</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ufo_832D9C58.DisplayName</x:t>
   </x:si>
   <x:si>
@@ -1056,6 +1095,27 @@
   </x:si>
   <x:si>
     <x:t>Assets/Miscellaneous</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ufo_66DF6E59.DisplayName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Documents/Images</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ufo_3DFEBE44.DisplayName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Characters</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Documents/Images/Characters</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ufo_20DB9DA3.DisplayName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entities/Characters</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1452,7 +1512,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D134"/>
+  <x:dimension ref="A1:D144"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -3030,49 +3090,163 @@
       <x:c r="A131" s="2" t="s">
         <x:v>327</x:v>
       </x:c>
-      <x:c r="B131" s="2" t="s">
-        <x:v>328</x:v>
-      </x:c>
+      <x:c r="B131" s="2" t="s"/>
       <x:c r="C131" s="2" t="s">
-        <x:v>329</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="D131" s="2" t="s"/>
     </x:row>
     <x:row r="132" spans="1:4">
       <x:c r="A132" s="2" t="s">
-        <x:v>330</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="B132" s="2" t="s">
-        <x:v>331</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="C132" s="2" t="s">
-        <x:v>332</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="D132" s="2" t="s"/>
     </x:row>
     <x:row r="133" spans="1:4">
       <x:c r="A133" s="2" t="s">
-        <x:v>333</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="B133" s="2" t="s">
-        <x:v>334</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="C133" s="2" t="s">
-        <x:v>335</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="D133" s="2" t="s"/>
     </x:row>
     <x:row r="134" spans="1:4">
       <x:c r="A134" s="2" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="B134" s="2" t="s"/>
+      <x:c r="C134" s="2" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="D134" s="2" t="s"/>
+    </x:row>
+    <x:row r="135" spans="1:4">
+      <x:c r="A135" s="2" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="B135" s="2" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="C135" s="2" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="D135" s="2" t="s"/>
+    </x:row>
+    <x:row r="136" spans="1:4">
+      <x:c r="A136" s="2" t="s">
         <x:v>336</x:v>
       </x:c>
-      <x:c r="B134" s="2" t="s">
+      <x:c r="B136" s="2" t="s"/>
+      <x:c r="C136" s="2" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="D136" s="2" t="s"/>
+    </x:row>
+    <x:row r="137" spans="1:4">
+      <x:c r="A137" s="2" t="s">
         <x:v>337</x:v>
       </x:c>
-      <x:c r="C134" s="2" t="s">
+      <x:c r="B137" s="2" t="s">
         <x:v>338</x:v>
       </x:c>
-      <x:c r="D134" s="2" t="s"/>
+      <x:c r="C137" s="2" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="D137" s="2" t="s"/>
+    </x:row>
+    <x:row r="138" spans="1:4">
+      <x:c r="A138" s="2" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="B138" s="2" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="C138" s="2" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="D138" s="2" t="s"/>
+    </x:row>
+    <x:row r="139" spans="1:4">
+      <x:c r="A139" s="2" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="B139" s="2" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C139" s="2" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="D139" s="2" t="s"/>
+    </x:row>
+    <x:row r="140" spans="1:4">
+      <x:c r="A140" s="2" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="B140" s="2" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="C140" s="2" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="D140" s="2" t="s"/>
+    </x:row>
+    <x:row r="141" spans="1:4">
+      <x:c r="A141" s="2" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="B141" s="2" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="C141" s="2" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="D141" s="2" t="s"/>
+    </x:row>
+    <x:row r="142" spans="1:4">
+      <x:c r="A142" s="2" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="B142" s="2" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="C142" s="2" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="D142" s="2" t="s"/>
+    </x:row>
+    <x:row r="143" spans="1:4">
+      <x:c r="A143" s="2" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="B143" s="2" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="C143" s="2" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="D143" s="2" t="s"/>
+    </x:row>
+    <x:row r="144" spans="1:4">
+      <x:c r="A144" s="2" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="B144" s="2" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="C144" s="2" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="D144" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Articy Project for test
</commit_message>
<xml_diff>
--- a/Assets/loc_All objects_en.xlsx
+++ b/Assets/loc_All objects_en.xlsx
@@ -454,7 +454,7 @@
     <x:t>Dlg_3EB04445.Text</x:t>
   </x:si>
   <x:si>
-    <x:t>Meu irmão,  &lt;color=#ffa61aff&gt;Jorrei&lt;/color&gt;, está no pátio de treinamento. Irei desafia-lo.</x:t>
+    <x:t>Meu irmão,  Jorrah, está no pátio de treinamento. Irei desafia-lo.</x:t>
   </x:si>
   <x:si>
     <x:t>Dlg_EE0B5AAB.DisplayName</x:t>
@@ -1031,10 +1031,10 @@
     <x:t>m_Jorrah.DisplayName</x:t>
   </x:si>
   <x:si>
-    <x:t>Jorrei</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Entities/Characters/Jorrei</x:t>
+    <x:t>Jorrah</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entities/Characters/Jorrah</x:t>
   </x:si>
   <x:si>
     <x:t>m_Jorrah.Text</x:t>

</xml_diff>